<commit_message>
Correccion del directorio de imagenes autorizadas
</commit_message>
<xml_diff>
--- a/wwwroot/UploadExcel/Prueba Lenel 1 dato.xlsx
+++ b/wwwroot/UploadExcel/Prueba Lenel 1 dato.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amejia/qa/Proy_Temperatura/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F262EF3-A235-2B4C-B07B-934A7D8FC3D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5667AF5D-F486-7748-9F26-0026C6EB8B5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38940" yWindow="1160" windowWidth="35160" windowHeight="14260" xr2:uid="{AD535384-A9A6-442B-B954-EFF58FBAA7DE}"/>
+    <workbookView xWindow="140" yWindow="12820" windowWidth="30280" windowHeight="7700" xr2:uid="{AD535384-A9A6-442B-B954-EFF58FBAA7DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>ID_lenel</t>
   </si>
@@ -75,7 +75,22 @@
     <t>QA Ingenieros Ltda</t>
   </si>
   <si>
-    <t>Inactivo(a)</t>
+    <t>MEJIA ARANGO</t>
+  </si>
+  <si>
+    <t>ISABELLA MARIA</t>
+  </si>
+  <si>
+    <t>T1019906212</t>
+  </si>
+  <si>
+    <t>Activo(a)</t>
+  </si>
+  <si>
+    <t>F Mejia</t>
+  </si>
+  <si>
+    <t>1019906212.jpg</t>
   </si>
 </sst>
 </file>
@@ -427,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F0A7BD-A803-4177-B68E-4C4999BDA747}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -443,6 +458,7 @@
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="35" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -488,10 +504,10 @@
         <v>8</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G2">
         <v>73146795</v>
@@ -501,6 +517,35 @@
       </c>
       <c r="I2" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3">
+        <v>1019906212</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se adiciona el control de fecha de inicio y final de autorizacion
</commit_message>
<xml_diff>
--- a/wwwroot/UploadExcel/Prueba Lenel 1 dato.xlsx
+++ b/wwwroot/UploadExcel/Prueba Lenel 1 dato.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amejia/qa/Proy_Temperatura/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5667AF5D-F486-7748-9F26-0026C6EB8B5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797F1B51-991B-1F41-8704-C87C2D678E17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="12820" windowWidth="30280" windowHeight="7700" xr2:uid="{AD535384-A9A6-442B-B954-EFF58FBAA7DE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>ID_lenel</t>
   </si>
@@ -91,15 +91,31 @@
   </si>
   <si>
     <t>1019906212.jpg</t>
+  </si>
+  <si>
+    <t>StartTime</t>
+  </si>
+  <si>
+    <t>EndTime</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="yyyy/mm/dd\ h:mm:ss"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -126,8 +142,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F0A7BD-A803-4177-B68E-4C4999BDA747}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -459,9 +476,11 @@
     <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="35" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
+    <col min="10" max="10" width="19.5" customWidth="1"/>
+    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,8 +508,14 @@
       <c r="I1" t="s">
         <v>10</v>
       </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -518,8 +543,14 @@
       <c r="I2" t="s">
         <v>9</v>
       </c>
+      <c r="J2" s="1">
+        <v>44018.999988425923</v>
+      </c>
+      <c r="K2" s="1">
+        <v>44171.999988425923</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -546,6 +577,12 @@
       </c>
       <c r="I3" t="s">
         <v>19</v>
+      </c>
+      <c r="J3" s="1">
+        <v>44018.999988425923</v>
+      </c>
+      <c r="K3" s="1">
+        <v>44171.999988425923</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios de las IP de servidores
</commit_message>
<xml_diff>
--- a/wwwroot/UploadExcel/Prueba Lenel 1 dato.xlsx
+++ b/wwwroot/UploadExcel/Prueba Lenel 1 dato.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amejia/qa/Proy_Temperatura/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797F1B51-991B-1F41-8704-C87C2D678E17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B373FD4-BFFA-AD40-8C8E-EA648A0BE00E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="12820" windowWidth="30280" windowHeight="7700" xr2:uid="{AD535384-A9A6-442B-B954-EFF58FBAA7DE}"/>
+    <workbookView xWindow="0" yWindow="13740" windowWidth="30280" windowHeight="10700" xr2:uid="{AD535384-A9A6-442B-B954-EFF58FBAA7DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>ID_lenel</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>EndTime</t>
+  </si>
+  <si>
+    <t>Inactivo(a)</t>
   </si>
 </sst>
 </file>
@@ -104,7 +107,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="yyyy/mm/dd\ h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd\ h:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -144,7 +147,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,7 +465,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -529,10 +532,10 @@
         <v>8</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G2">
         <v>73146795</v>

</xml_diff>